<commit_message>
Update fid.xlsx, sort fid.csv (#72)
</commit_message>
<xml_diff>
--- a/koapy/backend/kiwoom_open_api_plus/data/metadata/fid.xlsx
+++ b/koapy/backend/kiwoom_open_api_plus/data/metadata/fid.xlsx
@@ -1,26 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NXZT\Documents\git\koapy\koapy\backend\kiwoom_open_api_plus\data\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yunseong\Documents\git\koapy\koapy\backend\kiwoom_open_api_plus\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF58E0-6892-491C-B8A1-693F59463BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD827A55-19C3-45B3-A204-DB105F95D06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2475" windowWidth="35775" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="420" windowWidth="23700" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$796</definedName>
+    <definedName name="fid" localSheetId="0">Sheet1!$A$1:$B$796</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{80032ED4-A9FF-4407-A02F-65B5FA373DF5}" name="fid1" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\Yunseong\Documents\git\koapy\koapy\backend\kiwoom_open_api_plus\data\metadata\fid.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="735">
   <si>
     <t>대칭구분</t>
   </si>
@@ -1954,296 +1971,277 @@
     <t>평가손익</t>
   </si>
   <si>
+    <t>매도호가6</t>
+  </si>
+  <si>
+    <t>매도호가7</t>
+  </si>
+  <si>
+    <t>매도호가8</t>
+  </si>
+  <si>
+    <t>매도호가9</t>
+  </si>
+  <si>
+    <t>매도호가10</t>
+  </si>
+  <si>
+    <t>매수호가6</t>
+  </si>
+  <si>
+    <t>매수호가7</t>
+  </si>
+  <si>
+    <t>매수호가8</t>
+  </si>
+  <si>
+    <t>매수호가9</t>
+  </si>
+  <si>
+    <t>매수호가10</t>
+  </si>
+  <si>
+    <t>매도수량6</t>
+  </si>
+  <si>
+    <t>매도수량7</t>
+  </si>
+  <si>
+    <t>매도수량8</t>
+  </si>
+  <si>
+    <t>매도수량9</t>
+  </si>
+  <si>
+    <t>매도수량10</t>
+  </si>
+  <si>
+    <t>매수수량6</t>
+  </si>
+  <si>
+    <t>매수수량7</t>
+  </si>
+  <si>
+    <t>매수수량8</t>
+  </si>
+  <si>
+    <t>매수수량9</t>
+  </si>
+  <si>
+    <t>매수수량10</t>
+  </si>
+  <si>
+    <t>매도호가직전대비2</t>
+  </si>
+  <si>
+    <t>매도호가직전대비3</t>
+  </si>
+  <si>
+    <t>매도호가직전대비4</t>
+  </si>
+  <si>
+    <t>매도호가직전대비5</t>
+  </si>
+  <si>
+    <t>매도호가직전대비6</t>
+  </si>
+  <si>
+    <t>매도호가직전대비7</t>
+  </si>
+  <si>
+    <t>매도호가직전대비8</t>
+  </si>
+  <si>
+    <t>매도호가직전대비9</t>
+  </si>
+  <si>
+    <t>매도호가직전대비10</t>
+  </si>
+  <si>
+    <t>매수호가직전대비2</t>
+  </si>
+  <si>
+    <t>매수호가직전대비3</t>
+  </si>
+  <si>
+    <t>매수호가직전대비4</t>
+  </si>
+  <si>
+    <t>매수호가직전대비5</t>
+  </si>
+  <si>
+    <t>매수호가직전대비6</t>
+  </si>
+  <si>
+    <t>매수호가직전대비7</t>
+  </si>
+  <si>
+    <t>매수호가직전대비8</t>
+  </si>
+  <si>
+    <t>매수호가직전대비9</t>
+  </si>
+  <si>
+    <t>매수호가직전대비10</t>
+  </si>
+  <si>
+    <t>매도호가건수2</t>
+  </si>
+  <si>
+    <t>매도호가건수3</t>
+  </si>
+  <si>
+    <t>매도호가건수4</t>
+  </si>
+  <si>
+    <t>매도호가건수5</t>
+  </si>
+  <si>
+    <t>매수호가건수2</t>
+  </si>
+  <si>
+    <t>매수호가건수3</t>
+  </si>
+  <si>
+    <t>매수호가건수4</t>
+  </si>
+  <si>
+    <t>매수호가건수5</t>
+  </si>
+  <si>
+    <t>매도호가직전대비1</t>
+  </si>
+  <si>
+    <t>매수호가직전대비1</t>
+  </si>
+  <si>
+    <t>매도호가건수1</t>
+  </si>
+  <si>
+    <t>매수호가건수1</t>
+  </si>
+  <si>
+    <t>순매도잔량</t>
+  </si>
+  <si>
+    <t>매도비율</t>
+  </si>
+  <si>
+    <t>매도거래원색깔2</t>
+  </si>
+  <si>
+    <t>매도거래원색깔3</t>
+  </si>
+  <si>
+    <t>매도거래원색깔4</t>
+  </si>
+  <si>
+    <t>매도거래원색깔5</t>
+  </si>
+  <si>
+    <t>매수거래원색깔2</t>
+  </si>
+  <si>
+    <t>매수거래원색깔3</t>
+  </si>
+  <si>
+    <t>매수거래원색깔4</t>
+  </si>
+  <si>
+    <t>매수거래원색깔5</t>
+  </si>
+  <si>
+    <t>fid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>거래비용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매도호가6</t>
-  </si>
-  <si>
-    <t>매도호가7</t>
-  </si>
-  <si>
-    <t>매도호가8</t>
-  </si>
-  <si>
-    <t>매도호가9</t>
-  </si>
-  <si>
-    <t>매도호가10</t>
-  </si>
-  <si>
-    <t>매수호가6</t>
-  </si>
-  <si>
-    <t>매수호가7</t>
-  </si>
-  <si>
-    <t>매수호가8</t>
-  </si>
-  <si>
-    <t>매수호가9</t>
-  </si>
-  <si>
-    <t>매수호가10</t>
-  </si>
-  <si>
-    <t>매도수량6</t>
-  </si>
-  <si>
-    <t>매도수량7</t>
-  </si>
-  <si>
-    <t>매도수량8</t>
-  </si>
-  <si>
-    <t>매도수량9</t>
-  </si>
-  <si>
-    <t>매도수량10</t>
-  </si>
-  <si>
-    <t>매수수량6</t>
-  </si>
-  <si>
-    <t>매수수량7</t>
-  </si>
-  <si>
-    <t>매수수량8</t>
-  </si>
-  <si>
-    <t>매수수량9</t>
-  </si>
-  <si>
-    <t>매수수량10</t>
-  </si>
-  <si>
-    <t>매도호가직전대비2</t>
-  </si>
-  <si>
-    <t>매도호가직전대비3</t>
-  </si>
-  <si>
-    <t>매도호가직전대비4</t>
-  </si>
-  <si>
-    <t>매도호가직전대비5</t>
-  </si>
-  <si>
-    <t>매도호가직전대비6</t>
-  </si>
-  <si>
-    <t>매도호가직전대비7</t>
-  </si>
-  <si>
-    <t>매도호가직전대비8</t>
-  </si>
-  <si>
-    <t>매도호가직전대비9</t>
-  </si>
-  <si>
-    <t>매도호가직전대비10</t>
-  </si>
-  <si>
-    <t>매수호가직전대비2</t>
-  </si>
-  <si>
-    <t>매수호가직전대비3</t>
-  </si>
-  <si>
-    <t>매수호가직전대비4</t>
-  </si>
-  <si>
-    <t>매수호가직전대비5</t>
-  </si>
-  <si>
-    <t>매수호가직전대비6</t>
-  </si>
-  <si>
-    <t>매수호가직전대비7</t>
-  </si>
-  <si>
-    <t>매수호가직전대비8</t>
-  </si>
-  <si>
-    <t>매수호가직전대비9</t>
-  </si>
-  <si>
-    <t>매수호가직전대비10</t>
-  </si>
-  <si>
-    <t>매도호가건수2</t>
-  </si>
-  <si>
-    <t>매도호가건수3</t>
-  </si>
-  <si>
-    <t>매도호가건수4</t>
-  </si>
-  <si>
-    <t>매도호가건수5</t>
-  </si>
-  <si>
-    <t>매수호가건수2</t>
-  </si>
-  <si>
-    <t>매수호가건수3</t>
-  </si>
-  <si>
-    <t>매수호가건수4</t>
-  </si>
-  <si>
-    <t>매수호가건수5</t>
-  </si>
-  <si>
-    <t>매도호가직전대비1</t>
-  </si>
-  <si>
-    <t>매수호가직전대비1</t>
-  </si>
-  <si>
-    <t>매도호가건수1</t>
-  </si>
-  <si>
-    <t>매수호가건수1</t>
-  </si>
-  <si>
-    <t>순매도잔량</t>
-  </si>
-  <si>
-    <t>매도비율</t>
   </si>
   <si>
     <t>순매수수량증감</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>장운영구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>투자자별티커</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>외국계순매수추정합</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>외국계순매수변동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>매도거래원색깔1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매도거래원색깔2</t>
-  </si>
-  <si>
-    <t>매도거래원색깔3</t>
-  </si>
-  <si>
-    <t>매도거래원색깔4</t>
-  </si>
-  <si>
-    <t>매도거래원색깔5</t>
   </si>
   <si>
     <t>매수거래원색깔1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매수거래원색깔2</t>
-  </si>
-  <si>
-    <t>매수거래원색깔3</t>
-  </si>
-  <si>
-    <t>매수거래원색깔4</t>
-  </si>
-  <si>
-    <t>매수거래원색깔5</t>
   </si>
   <si>
     <t>장구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예상체결가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예상체결량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>예상체결가전일대비기호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>예상체결가전일대비등락율</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>전일거래량대비예상체결률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한도소진율</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>발행기관</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>차익순매수수량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>비차익거래매도금액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>비차익거래매수금액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비차익거래순매수금액</t>
   </si>
   <si>
     <t>비차익거래순매수수량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비차익거래순매수금액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LP회원사명1</t>
   </si>
   <si>
     <t>LP회원사명2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LP회원사명1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LP회원사명3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총매입가</t>
   </si>
   <si>
     <t>주문가능수량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>총매입가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거부사유</t>
+  </si>
+  <si>
+    <t>화면번호</t>
+  </si>
+  <si>
+    <t>당일실현손익_유가</t>
+  </si>
+  <si>
+    <t>당일실현손익률_유가</t>
+  </si>
+  <si>
+    <t>당일실현손익_신용</t>
+  </si>
+  <si>
+    <t>당일실현손익률_신용</t>
   </si>
 </sst>
 </file>
@@ -2292,28 +2290,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2324,6 +2301,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fid" connectionId="1" xr16:uid="{7F4E8FAF-74CB-4A85-8246-3655A8CAEB86}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2647,23 +2628,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B790"/>
+  <dimension ref="A1:B796"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
       <c r="B1" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2855,7 +2835,7 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>644</v>
+        <v>706</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2943,7 +2923,7 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2951,7 +2931,7 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2959,7 +2939,7 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2967,7 +2947,7 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2975,7 +2955,7 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3023,7 +3003,7 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -3031,7 +3011,7 @@
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -3039,7 +3019,7 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -3047,7 +3027,7 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -3055,7 +3035,7 @@
         <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -3103,7 +3083,7 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -3111,7 +3091,7 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -3119,7 +3099,7 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -3127,7 +3107,7 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -3135,7 +3115,7 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -3183,7 +3163,7 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -3191,7 +3171,7 @@
         <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -3199,7 +3179,7 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -3207,7 +3187,7 @@
         <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -3215,7 +3195,7 @@
         <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -3223,7 +3203,7 @@
         <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -3231,7 +3211,7 @@
         <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -3239,7 +3219,7 @@
         <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -3247,7 +3227,7 @@
         <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -3255,7 +3235,7 @@
         <v>85</v>
       </c>
       <c r="B75" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -3263,7 +3243,7 @@
         <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -3271,7 +3251,7 @@
         <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -3279,7 +3259,7 @@
         <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -3287,7 +3267,7 @@
         <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -3295,7 +3275,7 @@
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -3303,7 +3283,7 @@
         <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -3311,7 +3291,7 @@
         <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -3319,7 +3299,7 @@
         <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -3327,7 +3307,7 @@
         <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -3335,7 +3315,7 @@
         <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -3343,7 +3323,7 @@
         <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -3351,7 +3331,7 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -3359,7 +3339,7 @@
         <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -3367,7 +3347,7 @@
         <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -3375,7 +3355,7 @@
         <v>100</v>
       </c>
       <c r="B90" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -3383,7 +3363,7 @@
         <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -3391,7 +3371,7 @@
         <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -3399,7 +3379,7 @@
         <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -3407,7 +3387,7 @@
         <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -3415,7 +3395,7 @@
         <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -3423,7 +3403,7 @@
         <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -3431,7 +3411,7 @@
         <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -3439,7 +3419,7 @@
         <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -3447,7 +3427,7 @@
         <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -3455,7 +3435,7 @@
         <v>115</v>
       </c>
       <c r="B100" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -3567,7 +3547,7 @@
         <v>138</v>
       </c>
       <c r="B114" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -3575,7 +3555,7 @@
         <v>139</v>
       </c>
       <c r="B115" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -4127,7 +4107,7 @@
         <v>211</v>
       </c>
       <c r="B184" t="s">
-        <v>697</v>
+        <v>707</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -4151,7 +4131,7 @@
         <v>215</v>
       </c>
       <c r="B187" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -4159,7 +4139,7 @@
         <v>216</v>
       </c>
       <c r="B188" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -4399,7 +4379,7 @@
         <v>267</v>
       </c>
       <c r="B218" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -4407,7 +4387,7 @@
         <v>268</v>
       </c>
       <c r="B219" t="s">
-        <v>701</v>
+        <v>711</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -4423,7 +4403,7 @@
         <v>271</v>
       </c>
       <c r="B221" t="s">
-        <v>702</v>
+        <v>712</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -4431,7 +4411,7 @@
         <v>272</v>
       </c>
       <c r="B222" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
@@ -4439,7 +4419,7 @@
         <v>273</v>
       </c>
       <c r="B223" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -4447,7 +4427,7 @@
         <v>274</v>
       </c>
       <c r="B224" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -4455,7 +4435,7 @@
         <v>275</v>
       </c>
       <c r="B225" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -4463,7 +4443,7 @@
         <v>281</v>
       </c>
       <c r="B226" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -4471,7 +4451,7 @@
         <v>282</v>
       </c>
       <c r="B227" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -4479,7 +4459,7 @@
         <v>283</v>
       </c>
       <c r="B228" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -4487,7 +4467,7 @@
         <v>284</v>
       </c>
       <c r="B229" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -4495,7 +4475,7 @@
         <v>285</v>
       </c>
       <c r="B230" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
@@ -4503,7 +4483,7 @@
         <v>290</v>
       </c>
       <c r="B231" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -4511,7 +4491,7 @@
         <v>291</v>
       </c>
       <c r="B232" t="s">
-        <v>713</v>
+        <v>20</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -4519,7 +4499,7 @@
         <v>292</v>
       </c>
       <c r="B233" t="s">
-        <v>714</v>
+        <v>21</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -4663,7 +4643,7 @@
         <v>314</v>
       </c>
       <c r="B251" t="s">
-        <v>718</v>
+        <v>187</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -5135,7 +5115,7 @@
         <v>413</v>
       </c>
       <c r="B310" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
@@ -5599,7 +5579,7 @@
         <v>523</v>
       </c>
       <c r="B368" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
@@ -5631,7 +5611,7 @@
         <v>529</v>
       </c>
       <c r="B372" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
@@ -5671,7 +5651,7 @@
         <v>538</v>
       </c>
       <c r="B377" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
@@ -5703,7 +5683,7 @@
         <v>546</v>
       </c>
       <c r="B381" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
@@ -5935,7 +5915,7 @@
         <v>661</v>
       </c>
       <c r="B410" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
@@ -5951,7 +5931,7 @@
         <v>664</v>
       </c>
       <c r="B412" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
@@ -6484,2508 +6464,2550 @@
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>928</v>
+        <v>919</v>
       </c>
       <c r="B479" t="s">
-        <v>141</v>
+        <v>729</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="B480" t="s">
-        <v>138</v>
+        <v>730</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B481" t="s">
-        <v>382</v>
+        <v>141</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B482" t="s">
-        <v>383</v>
+        <v>138</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B483" t="s">
-        <v>729</v>
+        <v>382</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B484" t="s">
-        <v>728</v>
+        <v>383</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B485" t="s">
-        <v>384</v>
+        <v>727</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B486" t="s">
-        <v>385</v>
+        <v>728</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B487" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A488">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B488" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B489" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B490" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B491" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B492" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B493" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A494">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B494" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="B495" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B496" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="B497" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>951</v>
+        <v>946</v>
       </c>
       <c r="B498" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B499" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A500">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B500" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B501" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B502" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B503" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B504" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B505" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B506" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B507" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="B508" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B509" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="B510" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="B511" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>971</v>
+        <v>966</v>
       </c>
       <c r="B512" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A513">
-        <v>972</v>
+        <v>967</v>
       </c>
       <c r="B513" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A514">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B514" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B515" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B516" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A517">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B517" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A518">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B518" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A519">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B519" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A520">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B520" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A521">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B521" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A522">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B522" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A523">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B523" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A524">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B524" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A525">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B525" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A526">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B526" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A527">
-        <v>1000</v>
+        <v>984</v>
       </c>
       <c r="B527" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A528">
-        <v>1001</v>
+        <v>985</v>
       </c>
       <c r="B528" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A529">
-        <v>1002</v>
+        <v>990</v>
       </c>
       <c r="B529" t="s">
-        <v>428</v>
+        <v>731</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A530">
-        <v>1003</v>
+        <v>991</v>
       </c>
       <c r="B530" t="s">
-        <v>429</v>
+        <v>732</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A531">
-        <v>1004</v>
+        <v>992</v>
       </c>
       <c r="B531" t="s">
-        <v>430</v>
+        <v>733</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A532">
-        <v>1005</v>
+        <v>993</v>
       </c>
       <c r="B532" t="s">
-        <v>431</v>
+        <v>734</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A533">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="B533" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A534">
-        <v>1009</v>
+        <v>1001</v>
       </c>
       <c r="B534" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A535">
-        <v>1018</v>
+        <v>1002</v>
       </c>
       <c r="B535" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A536">
-        <v>1019</v>
+        <v>1003</v>
       </c>
       <c r="B536" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A537">
-        <v>1020</v>
+        <v>1004</v>
       </c>
       <c r="B537" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A538">
-        <v>1021</v>
+        <v>1005</v>
       </c>
       <c r="B538" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A539">
-        <v>1022</v>
+        <v>1006</v>
       </c>
       <c r="B539" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A540">
-        <v>1023</v>
+        <v>1009</v>
       </c>
       <c r="B540" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A541">
-        <v>1025</v>
+        <v>1018</v>
       </c>
       <c r="B541" t="s">
-        <v>15</v>
+        <v>434</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A542">
-        <v>1026</v>
+        <v>1019</v>
       </c>
       <c r="B542" t="s">
-        <v>16</v>
+        <v>435</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A543">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="B543" t="s">
-        <v>180</v>
+        <v>436</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A544">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="B544" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A545">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="B545" t="s">
-        <v>271</v>
+        <v>438</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A546">
-        <v>1033</v>
+        <v>1023</v>
       </c>
       <c r="B546" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A547">
-        <v>1034</v>
+        <v>1025</v>
       </c>
       <c r="B547" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A548">
-        <v>1035</v>
+        <v>1026</v>
       </c>
       <c r="B548" t="s">
-        <v>443</v>
+        <v>16</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A549">
-        <v>1036</v>
+        <v>1027</v>
       </c>
       <c r="B549" t="s">
-        <v>444</v>
+        <v>180</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A550">
-        <v>1037</v>
+        <v>1028</v>
       </c>
       <c r="B550" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A551">
-        <v>1040</v>
+        <v>1029</v>
       </c>
       <c r="B551" t="s">
-        <v>446</v>
+        <v>271</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A552">
-        <v>1041</v>
+        <v>1033</v>
       </c>
       <c r="B552" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A553">
-        <v>1042</v>
+        <v>1034</v>
       </c>
       <c r="B553" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A554">
-        <v>1043</v>
+        <v>1035</v>
       </c>
       <c r="B554" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A555">
-        <v>1044</v>
+        <v>1036</v>
       </c>
       <c r="B555" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A556">
-        <v>1045</v>
+        <v>1037</v>
       </c>
       <c r="B556" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="B557" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A558">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="B558" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A559">
-        <v>1048</v>
+        <v>1042</v>
       </c>
       <c r="B559" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A560">
-        <v>1049</v>
+        <v>1043</v>
       </c>
       <c r="B560" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A561">
-        <v>1051</v>
+        <v>1044</v>
       </c>
       <c r="B561" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A562">
-        <v>1052</v>
+        <v>1045</v>
       </c>
       <c r="B562" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A563">
-        <v>1054</v>
+        <v>1046</v>
       </c>
       <c r="B563" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A564">
-        <v>1055</v>
+        <v>1047</v>
       </c>
       <c r="B564" t="s">
-        <v>5</v>
+        <v>453</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A565">
-        <v>1056</v>
+        <v>1048</v>
       </c>
       <c r="B565" t="s">
-        <v>9</v>
+        <v>454</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A566">
-        <v>1058</v>
+        <v>1049</v>
       </c>
       <c r="B566" t="s">
-        <v>44</v>
+        <v>455</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A567">
-        <v>1059</v>
+        <v>1051</v>
       </c>
       <c r="B567" t="s">
-        <v>50</v>
+        <v>456</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A568">
-        <v>1060</v>
+        <v>1052</v>
       </c>
       <c r="B568" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A569">
-        <v>1063</v>
+        <v>1054</v>
       </c>
       <c r="B569" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A570">
-        <v>1065</v>
+        <v>1055</v>
       </c>
       <c r="B570" t="s">
-        <v>461</v>
+        <v>5</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A571">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="B571" t="s">
-        <v>462</v>
+        <v>9</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A572">
-        <v>1067</v>
+        <v>1058</v>
       </c>
       <c r="B572" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A573">
-        <v>1077</v>
+        <v>1059</v>
       </c>
       <c r="B573" t="s">
-        <v>463</v>
+        <v>50</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A574">
-        <v>1079</v>
+        <v>1060</v>
       </c>
       <c r="B574" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A575">
-        <v>1080</v>
+        <v>1063</v>
       </c>
       <c r="B575" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A576">
-        <v>1085</v>
+        <v>1065</v>
       </c>
       <c r="B576" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A577">
-        <v>1086</v>
+        <v>1066</v>
       </c>
       <c r="B577" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A578">
-        <v>1087</v>
+        <v>1067</v>
       </c>
       <c r="B578" t="s">
-        <v>468</v>
+        <v>22</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A579">
-        <v>1088</v>
+        <v>1077</v>
       </c>
       <c r="B579" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A580">
-        <v>1089</v>
+        <v>1079</v>
       </c>
       <c r="B580" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A581">
-        <v>1093</v>
+        <v>1080</v>
       </c>
       <c r="B581" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A582">
-        <v>1094</v>
+        <v>1085</v>
       </c>
       <c r="B582" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A583">
-        <v>1101</v>
+        <v>1086</v>
       </c>
       <c r="B583" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A584">
-        <v>1102</v>
+        <v>1087</v>
       </c>
       <c r="B584" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A585">
-        <v>1103</v>
+        <v>1088</v>
       </c>
       <c r="B585" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A586">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="B586" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A587">
-        <v>1105</v>
+        <v>1093</v>
       </c>
       <c r="B587" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588">
-        <v>1106</v>
+        <v>1094</v>
       </c>
       <c r="B588" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A589">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="B589" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="B590" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A591">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="B591" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A592">
-        <v>1111</v>
+        <v>1104</v>
       </c>
       <c r="B592" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593">
-        <v>1112</v>
+        <v>1105</v>
       </c>
       <c r="B593" t="s">
-        <v>7</v>
+        <v>477</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594">
-        <v>1113</v>
+        <v>1106</v>
       </c>
       <c r="B594" t="s">
-        <v>12</v>
+        <v>478</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595">
-        <v>1114</v>
+        <v>1107</v>
       </c>
       <c r="B595" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="B596" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597">
-        <v>1116</v>
+        <v>1109</v>
       </c>
       <c r="B597" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598">
-        <v>1117</v>
+        <v>1111</v>
       </c>
       <c r="B598" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="B599" t="s">
-        <v>487</v>
+        <v>7</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="B600" t="s">
-        <v>488</v>
+        <v>12</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="B601" t="s">
-        <v>271</v>
+        <v>483</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="B602" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="B603" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="B604" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="B605" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="B606" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A607">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="B607" t="s">
-        <v>494</v>
+        <v>271</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A608">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="B608" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="B609" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="B610" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="B611" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="B612" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="B613" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614">
-        <v>1134</v>
+        <v>1127</v>
       </c>
       <c r="B614" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A615">
-        <v>1135</v>
+        <v>1128</v>
       </c>
       <c r="B615" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="B616" t="s">
-        <v>135</v>
+        <v>497</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617">
-        <v>1137</v>
+        <v>1130</v>
       </c>
       <c r="B617" t="s">
-        <v>136</v>
+        <v>498</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618">
-        <v>1138</v>
+        <v>1131</v>
       </c>
       <c r="B618" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="B619" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A620">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="B620" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="B621" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="B622" t="s">
-        <v>508</v>
+        <v>135</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="B623" t="s">
-        <v>509</v>
+        <v>136</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="B624" t="s">
-        <v>8</v>
+        <v>503</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A625">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="B625" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A626">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="B626" t="s">
-        <v>187</v>
+        <v>505</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A627">
-        <v>1148</v>
+        <v>1141</v>
       </c>
       <c r="B627" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A628">
-        <v>1179</v>
+        <v>1142</v>
       </c>
       <c r="B628" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A629">
-        <v>1180</v>
+        <v>1143</v>
       </c>
       <c r="B629" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A630">
-        <v>1181</v>
+        <v>1144</v>
       </c>
       <c r="B630" t="s">
-        <v>514</v>
+        <v>8</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A631">
-        <v>1182</v>
+        <v>1145</v>
       </c>
       <c r="B631" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A632">
-        <v>1183</v>
+        <v>1146</v>
       </c>
       <c r="B632" t="s">
-        <v>516</v>
+        <v>187</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A633">
-        <v>1184</v>
+        <v>1148</v>
       </c>
       <c r="B633" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A634">
-        <v>1188</v>
+        <v>1179</v>
       </c>
       <c r="B634" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A635">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="B635" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A636">
-        <v>1201</v>
+        <v>1181</v>
       </c>
       <c r="B636" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A637">
-        <v>1202</v>
+        <v>1182</v>
       </c>
       <c r="B637" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A638">
-        <v>1203</v>
+        <v>1183</v>
       </c>
       <c r="B638" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A639">
-        <v>1204</v>
+        <v>1184</v>
       </c>
       <c r="B639" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A640">
-        <v>1205</v>
+        <v>1188</v>
       </c>
       <c r="B640" t="s">
-        <v>522</v>
+        <v>503</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641">
-        <v>1206</v>
+        <v>1189</v>
       </c>
       <c r="B641" t="s">
-        <v>523</v>
+        <v>504</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642">
-        <v>1215</v>
+        <v>1201</v>
       </c>
       <c r="B642" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643">
-        <v>1217</v>
+        <v>1202</v>
       </c>
       <c r="B643" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644">
-        <v>1221</v>
+        <v>1203</v>
       </c>
       <c r="B644" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645">
-        <v>1223</v>
+        <v>1204</v>
       </c>
       <c r="B645" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646">
-        <v>1224</v>
+        <v>1205</v>
       </c>
       <c r="B646" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647">
-        <v>1225</v>
+        <v>1206</v>
       </c>
       <c r="B647" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648">
-        <v>1236</v>
+        <v>1215</v>
       </c>
       <c r="B648" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649">
-        <v>1237</v>
+        <v>1217</v>
       </c>
       <c r="B649" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650">
-        <v>1238</v>
+        <v>1221</v>
       </c>
       <c r="B650" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651">
-        <v>1239</v>
+        <v>1223</v>
       </c>
       <c r="B651" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652">
-        <v>1341</v>
+        <v>1224</v>
       </c>
       <c r="B652" t="s">
-        <v>470</v>
+        <v>528</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653">
-        <v>1342</v>
+        <v>1225</v>
       </c>
       <c r="B653" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654">
-        <v>1344</v>
+        <v>1236</v>
       </c>
       <c r="B654" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655">
-        <v>1369</v>
+        <v>1237</v>
       </c>
       <c r="B655" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656">
-        <v>1370</v>
+        <v>1238</v>
       </c>
       <c r="B656" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A657">
-        <v>1371</v>
+        <v>1239</v>
       </c>
       <c r="B657" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A658">
-        <v>1396</v>
+        <v>1341</v>
       </c>
       <c r="B658" t="s">
-        <v>539</v>
+        <v>470</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A659">
-        <v>1400</v>
+        <v>1342</v>
       </c>
       <c r="B659" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A660">
-        <v>1401</v>
+        <v>1344</v>
       </c>
       <c r="B660" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A661">
-        <v>1402</v>
+        <v>1369</v>
       </c>
       <c r="B661" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A662">
-        <v>1404</v>
+        <v>1370</v>
       </c>
       <c r="B662" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A663">
-        <v>1405</v>
+        <v>1371</v>
       </c>
       <c r="B663" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A664">
-        <v>1406</v>
+        <v>1396</v>
       </c>
       <c r="B664" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A665">
-        <v>1408</v>
+        <v>1400</v>
       </c>
       <c r="B665" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A666">
-        <v>1409</v>
+        <v>1401</v>
       </c>
       <c r="B666" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A667">
-        <v>1410</v>
+        <v>1402</v>
       </c>
       <c r="B667" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A668">
-        <v>1411</v>
+        <v>1404</v>
       </c>
       <c r="B668" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A669">
-        <v>1412</v>
+        <v>1405</v>
       </c>
       <c r="B669" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A670">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="B670" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A671">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="B671" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A672">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="B672" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A673">
-        <v>1489</v>
+        <v>1410</v>
       </c>
       <c r="B673" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A674">
-        <v>1490</v>
+        <v>1411</v>
       </c>
       <c r="B674" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675">
-        <v>1600</v>
+        <v>1412</v>
       </c>
       <c r="B675" t="s">
-        <v>189</v>
+        <v>550</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676">
-        <v>1601</v>
+        <v>1413</v>
       </c>
       <c r="B676" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677">
-        <v>1604</v>
+        <v>1414</v>
       </c>
       <c r="B677" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678">
-        <v>1605</v>
+        <v>1415</v>
       </c>
       <c r="B678" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679">
-        <v>1608</v>
+        <v>1489</v>
       </c>
       <c r="B679" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680">
-        <v>1610</v>
+        <v>1490</v>
       </c>
       <c r="B680" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681">
-        <v>1611</v>
+        <v>1600</v>
       </c>
       <c r="B681" t="s">
-        <v>561</v>
+        <v>189</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682">
-        <v>1614</v>
+        <v>1601</v>
       </c>
       <c r="B682" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683">
-        <v>1630</v>
+        <v>1604</v>
       </c>
       <c r="B683" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684">
-        <v>1683</v>
+        <v>1605</v>
       </c>
       <c r="B684" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685">
-        <v>1684</v>
+        <v>1608</v>
       </c>
       <c r="B685" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686">
-        <v>1805</v>
+        <v>1610</v>
       </c>
       <c r="B686" t="s">
-        <v>473</v>
+        <v>560</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687">
-        <v>1811</v>
+        <v>1611</v>
       </c>
       <c r="B687" t="s">
-        <v>474</v>
+        <v>561</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688">
-        <v>1817</v>
+        <v>1614</v>
       </c>
       <c r="B688" t="s">
-        <v>475</v>
+        <v>562</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689">
-        <v>1823</v>
+        <v>1630</v>
       </c>
       <c r="B689" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690">
-        <v>1829</v>
+        <v>1683</v>
       </c>
       <c r="B690" t="s">
-        <v>476</v>
+        <v>564</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691">
-        <v>1835</v>
+        <v>1684</v>
       </c>
       <c r="B691" t="s">
-        <v>477</v>
+        <v>565</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692">
-        <v>1841</v>
+        <v>1805</v>
       </c>
       <c r="B692" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693">
-        <v>1847</v>
+        <v>1811</v>
       </c>
       <c r="B693" t="s">
-        <v>567</v>
+        <v>474</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694">
-        <v>1853</v>
+        <v>1817</v>
       </c>
       <c r="B694" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A695">
-        <v>1859</v>
+        <v>1823</v>
       </c>
       <c r="B695" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696">
-        <v>1965</v>
+        <v>1829</v>
       </c>
       <c r="B696" t="s">
-        <v>569</v>
+        <v>476</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697">
-        <v>1971</v>
+        <v>1835</v>
       </c>
       <c r="B697" t="s">
-        <v>570</v>
+        <v>477</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698">
-        <v>1977</v>
+        <v>1841</v>
       </c>
       <c r="B698" t="s">
-        <v>571</v>
+        <v>478</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699">
-        <v>3501</v>
+        <v>1847</v>
       </c>
       <c r="B699" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700">
-        <v>3502</v>
+        <v>1853</v>
       </c>
       <c r="B700" t="s">
-        <v>573</v>
+        <v>479</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701">
-        <v>3503</v>
+        <v>1859</v>
       </c>
       <c r="B701" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702">
-        <v>6001</v>
+        <v>1965</v>
       </c>
       <c r="B702" t="s">
-        <v>473</v>
+        <v>569</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703">
-        <v>6002</v>
+        <v>1971</v>
       </c>
       <c r="B703" t="s">
-        <v>474</v>
+        <v>570</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704">
-        <v>6003</v>
+        <v>1977</v>
       </c>
       <c r="B704" t="s">
-        <v>475</v>
+        <v>571</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705">
-        <v>6004</v>
+        <v>3501</v>
       </c>
       <c r="B705" t="s">
-        <v>476</v>
+        <v>572</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706">
-        <v>6005</v>
+        <v>3502</v>
       </c>
       <c r="B706" t="s">
-        <v>477</v>
+        <v>573</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707">
-        <v>6006</v>
+        <v>3503</v>
       </c>
       <c r="B707" t="s">
-        <v>478</v>
+        <v>574</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708">
-        <v>6007</v>
+        <v>6001</v>
       </c>
       <c r="B708" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A709">
-        <v>6008</v>
+        <v>6002</v>
       </c>
       <c r="B709" t="s">
-        <v>568</v>
+        <v>474</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710">
-        <v>6009</v>
+        <v>6003</v>
       </c>
       <c r="B710" t="s">
-        <v>569</v>
+        <v>475</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711">
-        <v>6010</v>
+        <v>6004</v>
       </c>
       <c r="B711" t="s">
-        <v>570</v>
+        <v>476</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712">
-        <v>6012</v>
+        <v>6005</v>
       </c>
       <c r="B712" t="s">
-        <v>567</v>
+        <v>477</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713">
-        <v>6013</v>
+        <v>6006</v>
       </c>
       <c r="B713" t="s">
-        <v>566</v>
+        <v>478</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714">
-        <v>6014</v>
+        <v>6007</v>
       </c>
       <c r="B714" t="s">
-        <v>571</v>
+        <v>479</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715">
-        <v>6021</v>
+        <v>6008</v>
       </c>
       <c r="B715" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716">
-        <v>6022</v>
+        <v>6009</v>
       </c>
       <c r="B716" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717">
-        <v>6023</v>
+        <v>6010</v>
       </c>
       <c r="B717" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718">
-        <v>6024</v>
+        <v>6012</v>
       </c>
       <c r="B718" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719">
-        <v>6025</v>
+        <v>6013</v>
       </c>
       <c r="B719" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720">
-        <v>6026</v>
+        <v>6014</v>
       </c>
       <c r="B720" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A721">
-        <v>6027</v>
+        <v>6021</v>
       </c>
       <c r="B721" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A722">
-        <v>6028</v>
+        <v>6022</v>
       </c>
       <c r="B722" t="s">
-        <v>506</v>
+        <v>576</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A723">
-        <v>6029</v>
+        <v>6023</v>
       </c>
       <c r="B723" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A724">
-        <v>6030</v>
+        <v>6024</v>
       </c>
       <c r="B724" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725">
-        <v>6032</v>
+        <v>6025</v>
       </c>
       <c r="B725" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726">
-        <v>6033</v>
+        <v>6026</v>
       </c>
       <c r="B726" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727">
-        <v>6034</v>
+        <v>6027</v>
       </c>
       <c r="B727" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728">
-        <v>8000</v>
+        <v>6028</v>
       </c>
       <c r="B728" t="s">
-        <v>568</v>
+        <v>506</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729">
-        <v>8002</v>
+        <v>6029</v>
       </c>
       <c r="B729" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A730">
-        <v>8003</v>
+        <v>6030</v>
       </c>
       <c r="B730" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A731">
-        <v>8004</v>
+        <v>6032</v>
       </c>
       <c r="B731" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A732">
-        <v>8005</v>
+        <v>6033</v>
       </c>
       <c r="B732" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A733">
-        <v>8006</v>
+        <v>6034</v>
       </c>
       <c r="B733" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A734">
-        <v>8007</v>
+        <v>8000</v>
       </c>
       <c r="B734" t="s">
-        <v>592</v>
+        <v>568</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A735">
-        <v>8008</v>
+        <v>8002</v>
       </c>
       <c r="B735" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736">
-        <v>8018</v>
+        <v>8003</v>
       </c>
       <c r="B736" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737">
-        <v>8019</v>
+        <v>8004</v>
       </c>
       <c r="B737" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738">
-        <v>8020</v>
+        <v>8005</v>
       </c>
       <c r="B738" t="s">
-        <v>381</v>
+        <v>590</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739">
-        <v>8021</v>
+        <v>8006</v>
       </c>
       <c r="B739" t="s">
-        <v>380</v>
+        <v>591</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740">
-        <v>8040</v>
+        <v>8007</v>
       </c>
       <c r="B740" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741">
-        <v>8041</v>
+        <v>8008</v>
       </c>
       <c r="B741" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742">
-        <v>8042</v>
+        <v>8018</v>
       </c>
       <c r="B742" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A743">
-        <v>9001</v>
+        <v>8019</v>
       </c>
       <c r="B743" t="s">
-        <v>174</v>
+        <v>595</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744">
-        <v>9004</v>
+        <v>8020</v>
       </c>
       <c r="B744" t="s">
-        <v>599</v>
+        <v>381</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745">
-        <v>9019</v>
+        <v>8021</v>
       </c>
       <c r="B745" t="s">
-        <v>600</v>
+        <v>380</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746">
-        <v>9026</v>
+        <v>8040</v>
       </c>
       <c r="B746" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747">
-        <v>9201</v>
+        <v>8041</v>
       </c>
       <c r="B747" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748">
-        <v>9203</v>
+        <v>8042</v>
       </c>
       <c r="B748" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749">
-        <v>9205</v>
+        <v>9001</v>
       </c>
       <c r="B749" t="s">
-        <v>604</v>
+        <v>174</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750">
-        <v>10010</v>
+        <v>9004</v>
       </c>
       <c r="B750" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751">
-        <v>10011</v>
+        <v>9019</v>
       </c>
       <c r="B751" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A752">
-        <v>10012</v>
+        <v>9026</v>
       </c>
       <c r="B752" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A753">
-        <v>10013</v>
+        <v>9201</v>
       </c>
       <c r="B753" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A754">
-        <v>10023</v>
+        <v>9203</v>
       </c>
       <c r="B754" t="s">
-        <v>20</v>
+        <v>603</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755">
-        <v>10024</v>
+        <v>9205</v>
       </c>
       <c r="B755" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A756">
-        <v>10025</v>
+        <v>10010</v>
       </c>
       <c r="B756" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757">
-        <v>10041</v>
+        <v>10011</v>
       </c>
       <c r="B757" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A758">
-        <v>10042</v>
+        <v>10012</v>
       </c>
       <c r="B758" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759">
-        <v>10043</v>
+        <v>10013</v>
       </c>
       <c r="B759" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A760">
-        <v>10044</v>
+        <v>10023</v>
       </c>
       <c r="B760" t="s">
-        <v>614</v>
+        <v>20</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A761">
-        <v>10045</v>
+        <v>10024</v>
       </c>
       <c r="B761" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A762">
-        <v>10051</v>
+        <v>10025</v>
       </c>
       <c r="B762" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A763">
-        <v>10052</v>
+        <v>10041</v>
       </c>
       <c r="B763" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A764">
-        <v>10053</v>
+        <v>10042</v>
       </c>
       <c r="B764" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A765">
-        <v>10054</v>
+        <v>10043</v>
       </c>
       <c r="B765" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A766">
-        <v>10055</v>
+        <v>10044</v>
       </c>
       <c r="B766" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A767">
-        <v>10061</v>
+        <v>10045</v>
       </c>
       <c r="B767" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A768">
-        <v>10062</v>
+        <v>10051</v>
       </c>
       <c r="B768" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A769">
-        <v>10063</v>
+        <v>10052</v>
       </c>
       <c r="B769" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A770">
-        <v>10064</v>
+        <v>10053</v>
       </c>
       <c r="B770" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A771">
-        <v>10065</v>
+        <v>10054</v>
       </c>
       <c r="B771" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A772">
-        <v>10071</v>
+        <v>10055</v>
       </c>
       <c r="B772" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773">
-        <v>10072</v>
+        <v>10061</v>
       </c>
       <c r="B773" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A774">
-        <v>10073</v>
+        <v>10062</v>
       </c>
       <c r="B774" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A775">
-        <v>10074</v>
+        <v>10063</v>
       </c>
       <c r="B775" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A776">
-        <v>10075</v>
+        <v>10064</v>
       </c>
       <c r="B776" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A777">
-        <v>10081</v>
+        <v>10065</v>
       </c>
       <c r="B777" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A778">
-        <v>10082</v>
+        <v>10071</v>
       </c>
       <c r="B778" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A779">
-        <v>10083</v>
+        <v>10072</v>
       </c>
       <c r="B779" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A780">
-        <v>10084</v>
+        <v>10073</v>
       </c>
       <c r="B780" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A781">
-        <v>10085</v>
+        <v>10074</v>
       </c>
       <c r="B781" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A782">
-        <v>10091</v>
+        <v>10075</v>
       </c>
       <c r="B782" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A783">
-        <v>10092</v>
+        <v>10081</v>
       </c>
       <c r="B783" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A784">
-        <v>10093</v>
+        <v>10082</v>
       </c>
       <c r="B784" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A785">
-        <v>10094</v>
+        <v>10083</v>
       </c>
       <c r="B785" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A786">
-        <v>10095</v>
+        <v>10084</v>
       </c>
       <c r="B786" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A787">
-        <v>10121</v>
+        <v>10085</v>
       </c>
       <c r="B787" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A788">
-        <v>10125</v>
+        <v>10091</v>
       </c>
       <c r="B788" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789">
-        <v>13000</v>
+        <v>10092</v>
       </c>
       <c r="B789" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A790">
+        <v>10093</v>
+      </c>
+      <c r="B790" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A791">
+        <v>10094</v>
+      </c>
+      <c r="B791" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A792">
+        <v>10095</v>
+      </c>
+      <c r="B792" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A793">
+        <v>10121</v>
+      </c>
+      <c r="B793" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A794">
+        <v>10125</v>
+      </c>
+      <c r="B794" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A795">
+        <v>13000</v>
+      </c>
+      <c r="B795" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A796">
         <v>28669</v>
       </c>
-      <c r="B790" t="s">
+      <c r="B796" t="s">
         <v>333</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A185 A190:A217 A238:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A186:A189">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>